<commit_message>
temp change to canis filters
</commit_message>
<xml_diff>
--- a/dependencies/brucella/canis/script_dependents/Filtered_Regions.xlsx
+++ b/dependencies/brucella/canis/script_dependents/Filtered_Regions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/root/TStuber/Results/brucella/canis/script_dependents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\TStuber\Results\brucella\canis\script_dependents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244E371D-A7E7-664F-8E91-8A42C22F1430}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="4860" windowWidth="25880" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14760" yWindow="4860" windowWidth="25875" windowHeight="16875" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NC_010103.1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>629454-630269</t>
   </si>
@@ -86,12 +85,15 @@
   </si>
   <si>
     <t>1109431</t>
+  </si>
+  <si>
+    <t>626896-662986</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1121,8 +1123,8 @@
     <cellStyle name="Linked Cell" xfId="142" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="138" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="171" xr:uid="{00000000-0005-0000-0000-000011010000}"/>
-    <cellStyle name="Note 2" xfId="172" xr:uid="{00000000-0005-0000-0000-000012010000}"/>
+    <cellStyle name="Normal 2" xfId="171"/>
+    <cellStyle name="Note 2" xfId="172"/>
     <cellStyle name="Output" xfId="140" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="131" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="146" builtinId="25" customBuiltin="1"/>
@@ -1462,20 +1464,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="44.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1495,57 +1497,57 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -1557,20 +1559,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="44.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1590,19 +1592,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>